<commit_message>
merge eclipse (on y croit)
</commit_message>
<xml_diff>
--- a/GestiBank/PATHS.xlsx
+++ b/GestiBank/PATHS.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="73">
   <si>
     <t>VERBE</t>
   </si>
@@ -207,12 +207,6 @@
     <t>&lt;site&gt;/comptes/client/{id}</t>
   </si>
   <si>
-    <t>&lt;site&gt;/notifications/client/{id}</t>
-  </si>
-  <si>
-    <t>getNotifications(clientID)</t>
-  </si>
-  <si>
     <t>&lt;site&gt;/operations/compte/{id}</t>
   </si>
   <si>
@@ -226,6 +220,21 @@
   </si>
   <si>
     <t>&lt;site&gt;/login</t>
+  </si>
+  <si>
+    <t>&lt;site&gt;/notifications/{id}</t>
+  </si>
+  <si>
+    <t>deleteNotification(id)</t>
+  </si>
+  <si>
+    <t>void</t>
+  </si>
+  <si>
+    <t>addNotificationToClient(clientId)</t>
+  </si>
+  <si>
+    <t>getNotificationsByClient(clientID)</t>
   </si>
 </sst>
 </file>
@@ -305,8 +314,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:E28" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="A1:E28"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:E31" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A1:E31"/>
   <sortState ref="A2:E28">
     <sortCondition ref="E1:E28"/>
   </sortState>
@@ -608,10 +617,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E27"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -930,29 +939,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>8</v>
-      </c>
-      <c r="B20" t="s">
-        <v>63</v>
-      </c>
-      <c r="C20" t="s">
-        <v>64</v>
-      </c>
-      <c r="D20" t="s">
-        <v>45</v>
-      </c>
-      <c r="E20" t="s">
-        <v>10</v>
-      </c>
-    </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>8</v>
       </c>
       <c r="B21" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C21" t="s">
         <v>46</v>
@@ -986,7 +978,7 @@
         <v>12</v>
       </c>
       <c r="B23" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C23" t="s">
         <v>34</v>
@@ -1003,7 +995,7 @@
         <v>20</v>
       </c>
       <c r="B24" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C24" t="s">
         <v>37</v>
@@ -1020,7 +1012,7 @@
         <v>8</v>
       </c>
       <c r="B25" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C25" t="s">
         <v>38</v>
@@ -1037,7 +1029,7 @@
         <v>12</v>
       </c>
       <c r="B26" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C26" t="s">
         <v>31</v>
@@ -1054,7 +1046,7 @@
         <v>12</v>
       </c>
       <c r="B27" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C27" t="s">
         <v>50</v>
@@ -1064,6 +1056,57 @@
       </c>
       <c r="E27" t="s">
         <v>32</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>14</v>
+      </c>
+      <c r="B29" t="s">
+        <v>68</v>
+      </c>
+      <c r="C29" t="s">
+        <v>69</v>
+      </c>
+      <c r="D29" t="s">
+        <v>70</v>
+      </c>
+      <c r="E29" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>12</v>
+      </c>
+      <c r="B30" t="s">
+        <v>68</v>
+      </c>
+      <c r="C30" t="s">
+        <v>71</v>
+      </c>
+      <c r="D30" t="s">
+        <v>70</v>
+      </c>
+      <c r="E30" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>8</v>
+      </c>
+      <c r="B31" t="s">
+        <v>68</v>
+      </c>
+      <c r="C31" t="s">
+        <v>72</v>
+      </c>
+      <c r="D31" t="s">
+        <v>45</v>
+      </c>
+      <c r="E31" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
♫ c'est la java bleue ♪
</commit_message>
<xml_diff>
--- a/GestiBank/PATHS.xlsx
+++ b/GestiBank/PATHS.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="82">
   <si>
     <t>VERBE</t>
   </si>
@@ -51,9 +51,6 @@
     <t>CLIENT</t>
   </si>
   <si>
-    <t>listClients()</t>
-  </si>
-  <si>
     <t>POST</t>
   </si>
   <si>
@@ -63,30 +60,12 @@
     <t>DELETE</t>
   </si>
   <si>
-    <t>deleteConseiller()</t>
-  </si>
-  <si>
     <t>Void</t>
   </si>
   <si>
-    <t>getConseillerByName(name)</t>
-  </si>
-  <si>
-    <t>getConseillerById(id)</t>
-  </si>
-  <si>
-    <t>createConseiller(conseiller)</t>
-  </si>
-  <si>
     <t>PUT</t>
   </si>
   <si>
-    <t>updateConseiller(conseiller)</t>
-  </si>
-  <si>
-    <t>deleteConseiller(id)</t>
-  </si>
-  <si>
     <t>List&lt;Demande&gt;</t>
   </si>
   <si>
@@ -165,24 +144,9 @@
     <t>sendDemande(demande, conseillerID)</t>
   </si>
   <si>
-    <t>listAllUsers(type)</t>
-  </si>
-  <si>
     <t>login(username, password)</t>
   </si>
   <si>
-    <t>&lt;site&gt;/users</t>
-  </si>
-  <si>
-    <t>&lt;site&gt;/conseillers/{conseiller}</t>
-  </si>
-  <si>
-    <t>&lt;site&gt;/conseillers/{id}</t>
-  </si>
-  <si>
-    <t>&lt;site&gt;/conseillers/{name}</t>
-  </si>
-  <si>
     <t>&lt;site&gt;/demandes</t>
   </si>
   <si>
@@ -198,9 +162,6 @@
     <t>&lt;site&gt;/conseillers/{id}/clients/{id}</t>
   </si>
   <si>
-    <t>&lt;site&gt;/conseillers/{id}/clients</t>
-  </si>
-  <si>
     <t>&lt;site&gt;/comptes/{id}</t>
   </si>
   <si>
@@ -222,12 +183,6 @@
     <t>&lt;site&gt;/login</t>
   </si>
   <si>
-    <t>&lt;site&gt;/notifications/{id}</t>
-  </si>
-  <si>
-    <t>deleteNotification(id)</t>
-  </si>
-  <si>
     <t>void</t>
   </si>
   <si>
@@ -235,13 +190,85 @@
   </si>
   <si>
     <t>getNotificationsByClient(clientID)</t>
+  </si>
+  <si>
+    <t>boolean</t>
+  </si>
+  <si>
+    <t>deleteNotification(notificationId)</t>
+  </si>
+  <si>
+    <t>&lt;site&gt;/notifications/{notificationId}</t>
+  </si>
+  <si>
+    <t>&lt;site&gt;/notifications/{clientId}</t>
+  </si>
+  <si>
+    <t>&lt;site&gt;/conseillers</t>
+  </si>
+  <si>
+    <t>getAll()</t>
+  </si>
+  <si>
+    <t>&lt;site&gt;/conseillers/{recherche}</t>
+  </si>
+  <si>
+    <t>&lt;site&gt;/conseillers/{matricule}/clients</t>
+  </si>
+  <si>
+    <t>getClientsFromConseiller(String matricule)</t>
+  </si>
+  <si>
+    <t>getConseillerByNameOrMatricule(String recherche)</t>
+  </si>
+  <si>
+    <t>updateConseiller(Conseiller conseiller)</t>
+  </si>
+  <si>
+    <t>WS conseiller</t>
+  </si>
+  <si>
+    <t>WS</t>
+  </si>
+  <si>
+    <t>addConseiller(Conseiller conseiller)</t>
+  </si>
+  <si>
+    <t>&lt;site&gt;/conseillers/{matricule}</t>
+  </si>
+  <si>
+    <t>deleteConseiller(String matricule)</t>
+  </si>
+  <si>
+    <t>&lt;site&gt;/conseillers/{matricule}/inscriptions</t>
+  </si>
+  <si>
+    <t>getInscriptionsFromConseiller(String matricule)</t>
+  </si>
+  <si>
+    <t>List&lt;DemandeInscription&gt;</t>
+  </si>
+  <si>
+    <t>&lt;site&gt;/clients/{id}/conseiller</t>
+  </si>
+  <si>
+    <t>updateConseiller(String newConseillerMatricule)</t>
+  </si>
+  <si>
+    <t>WS client</t>
+  </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>Test</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -255,6 +282,13 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -278,9 +312,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -314,17 +349,19 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:E31" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="A1:E31"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:G32" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A1:G32"/>
   <sortState ref="A2:E28">
     <sortCondition ref="E1:E28"/>
   </sortState>
-  <tableColumns count="5">
+  <tableColumns count="7">
     <tableColumn id="1" name="VERBE"/>
     <tableColumn id="2" name="PATH"/>
     <tableColumn id="3" name="METHODE"/>
     <tableColumn id="4" name="RETURN"/>
     <tableColumn id="5" name="COTE"/>
+    <tableColumn id="6" name="WS"/>
+    <tableColumn id="7" name="Test"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -617,10 +654,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -633,7 +670,7 @@
     <col min="6" max="6" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -649,186 +686,213 @@
       <c r="E1" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="C2" t="s">
-        <v>49</v>
+        <v>63</v>
       </c>
       <c r="D2" t="s">
         <v>5</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
+        <v>69</v>
+      </c>
+      <c r="G2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3" t="s">
+        <v>69</v>
+      </c>
+      <c r="G3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D4" t="s">
         <v>12</v>
-      </c>
-      <c r="B4" t="s">
-        <v>52</v>
-      </c>
-      <c r="C4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" t="s">
-        <v>13</v>
       </c>
       <c r="E4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>53</v>
+        <v>65</v>
       </c>
       <c r="C5" t="s">
-        <v>18</v>
+        <v>66</v>
       </c>
       <c r="D5" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="E5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+      <c r="F5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="C6" t="s">
-        <v>15</v>
+        <v>71</v>
       </c>
       <c r="D6" t="s">
-        <v>16</v>
+        <v>55</v>
       </c>
       <c r="E6" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>54</v>
+        <v>72</v>
       </c>
       <c r="C7" t="s">
-        <v>17</v>
+        <v>73</v>
       </c>
       <c r="D7" t="s">
-        <v>13</v>
+        <v>55</v>
       </c>
       <c r="E7" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F7" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>53</v>
+        <v>74</v>
       </c>
       <c r="C8" t="s">
-        <v>21</v>
+        <v>75</v>
       </c>
       <c r="D8" t="s">
-        <v>13</v>
-      </c>
-      <c r="E8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+      <c r="F8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>53</v>
+        <v>77</v>
       </c>
       <c r="C9" t="s">
-        <v>22</v>
+        <v>78</v>
       </c>
       <c r="D9" t="s">
-        <v>16</v>
-      </c>
-      <c r="E9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" t="s">
         <v>55</v>
       </c>
-      <c r="C10" t="s">
-        <v>25</v>
-      </c>
-      <c r="D10" t="s">
-        <v>23</v>
-      </c>
-      <c r="E10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F9" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="C11" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="D11" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="E11" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="C12" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="D12" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="E12" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B13" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="C13" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="D13" t="s">
         <v>16</v>
@@ -837,72 +901,55 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="C14" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="D14" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="E14" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="C15" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="D15" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E15" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B16" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="C16" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="D16" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="E16" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>8</v>
-      </c>
-      <c r="B17" t="s">
-        <v>40</v>
-      </c>
-      <c r="C17" t="s">
-        <v>41</v>
-      </c>
-      <c r="D17" t="s">
-        <v>35</v>
-      </c>
-      <c r="E17" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -910,13 +957,13 @@
         <v>8</v>
       </c>
       <c r="B18" t="s">
-        <v>62</v>
+        <v>33</v>
       </c>
       <c r="C18" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="D18" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="E18" t="s">
         <v>10</v>
@@ -927,47 +974,47 @@
         <v>8</v>
       </c>
       <c r="B19" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="C19" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="D19" t="s">
-        <v>44</v>
+        <v>9</v>
       </c>
       <c r="E19" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>8</v>
       </c>
-      <c r="B21" t="s">
-        <v>63</v>
-      </c>
-      <c r="C21" t="s">
-        <v>46</v>
-      </c>
-      <c r="D21" t="s">
-        <v>47</v>
-      </c>
-      <c r="E21" t="s">
+      <c r="B20" t="s">
+        <v>48</v>
+      </c>
+      <c r="C20" t="s">
+        <v>36</v>
+      </c>
+      <c r="D20" t="s">
+        <v>37</v>
+      </c>
+      <c r="E20" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B22" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C22" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="D22" t="s">
-        <v>16</v>
+        <v>40</v>
       </c>
       <c r="E22" t="s">
         <v>10</v>
@@ -975,118 +1022,118 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B23" t="s">
-        <v>64</v>
+        <v>43</v>
       </c>
       <c r="C23" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="D23" t="s">
-        <v>35</v>
+        <v>14</v>
       </c>
       <c r="E23" t="s">
-        <v>36</v>
+        <v>10</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="B24" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="C24" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="D24" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="E24" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="B25" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="C25" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="D25" t="s">
-        <v>35</v>
+        <v>14</v>
       </c>
       <c r="E25" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B26" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="C26" t="s">
         <v>31</v>
       </c>
       <c r="D26" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E26" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B27" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
       <c r="C27" t="s">
-        <v>50</v>
+        <v>24</v>
       </c>
       <c r="D27" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="E27" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>14</v>
-      </c>
-      <c r="B29" t="s">
-        <v>68</v>
-      </c>
-      <c r="C29" t="s">
-        <v>69</v>
-      </c>
-      <c r="D29" t="s">
-        <v>70</v>
-      </c>
-      <c r="E29" t="s">
-        <v>10</v>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>11</v>
+      </c>
+      <c r="B28" t="s">
+        <v>54</v>
+      </c>
+      <c r="C28" t="s">
+        <v>42</v>
+      </c>
+      <c r="D28" t="s">
+        <v>26</v>
+      </c>
+      <c r="E28" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B30" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="C30" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="D30" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="E30" t="s">
         <v>10</v>
@@ -1094,18 +1141,35 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>11</v>
+      </c>
+      <c r="B31" t="s">
+        <v>61</v>
+      </c>
+      <c r="C31" t="s">
+        <v>56</v>
+      </c>
+      <c r="D31" t="s">
+        <v>58</v>
+      </c>
+      <c r="E31" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>8</v>
       </c>
-      <c r="B31" t="s">
-        <v>68</v>
-      </c>
-      <c r="C31" t="s">
-        <v>72</v>
-      </c>
-      <c r="D31" t="s">
-        <v>45</v>
-      </c>
-      <c r="E31" t="s">
+      <c r="B32" t="s">
+        <v>61</v>
+      </c>
+      <c r="C32" t="s">
+        <v>57</v>
+      </c>
+      <c r="D32" t="s">
+        <v>38</v>
+      </c>
+      <c r="E32" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Problème d'accents lors du passage par WS résolu
il fallait ajouter les options dans post et put pour avoir utf-8 dans le header du fichier json que l'on envoie depuis angular
</commit_message>
<xml_diff>
--- a/GestiBank/PATHS.xlsx
+++ b/GestiBank/PATHS.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19001"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\base\GestiBank\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="60" windowWidth="28515" windowHeight="12840"/>
+    <workbookView xWindow="120" yWindow="60" windowWidth="28512" windowHeight="12840"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="77">
   <si>
     <t>VERBE</t>
   </si>
@@ -51,9 +56,6 @@
     <t>CLIENT</t>
   </si>
   <si>
-    <t>listClients()</t>
-  </si>
-  <si>
     <t>POST</t>
   </si>
   <si>
@@ -63,54 +65,15 @@
     <t>DELETE</t>
   </si>
   <si>
-    <t>deleteConseiller()</t>
-  </si>
-  <si>
     <t>Void</t>
   </si>
   <si>
-    <t>getConseillerByName(name)</t>
-  </si>
-  <si>
-    <t>getConseillerById(id)</t>
-  </si>
-  <si>
-    <t>createConseiller(conseiller)</t>
-  </si>
-  <si>
     <t>PUT</t>
   </si>
   <si>
-    <t>updateConseiller(conseiller)</t>
-  </si>
-  <si>
-    <t>deleteConseiller(id)</t>
-  </si>
-  <si>
-    <t>List&lt;Demande&gt;</t>
-  </si>
-  <si>
-    <t>getUnassignedDemandesInscription(bool)</t>
-  </si>
-  <si>
-    <t>getAllDemandesInscription()</t>
-  </si>
-  <si>
-    <t>getDemandesInscriptionByStatus(string)</t>
-  </si>
-  <si>
     <t>Demande</t>
   </si>
   <si>
-    <t>updateDemandeInscription(demande)</t>
-  </si>
-  <si>
-    <t>assignDemandeInscription(conseillerId, demandeId)</t>
-  </si>
-  <si>
-    <t>assignClient(conseiller)</t>
-  </si>
-  <si>
     <t>createDemandeInscription(personne)</t>
   </si>
   <si>
@@ -135,9 +98,6 @@
     <t>getClientByName(name)</t>
   </si>
   <si>
-    <t>ADMIN/CONSEILLER</t>
-  </si>
-  <si>
     <t>&lt;site&gt;/client/{id}</t>
   </si>
   <si>
@@ -165,42 +125,12 @@
     <t>sendDemande(demande, conseillerID)</t>
   </si>
   <si>
-    <t>listAllUsers(type)</t>
-  </si>
-  <si>
     <t>login(username, password)</t>
   </si>
   <si>
-    <t>&lt;site&gt;/users</t>
-  </si>
-  <si>
-    <t>&lt;site&gt;/conseillers/{conseiller}</t>
-  </si>
-  <si>
-    <t>&lt;site&gt;/conseillers/{id}</t>
-  </si>
-  <si>
-    <t>&lt;site&gt;/conseillers/{name}</t>
-  </si>
-  <si>
     <t>&lt;site&gt;/demandes</t>
   </si>
   <si>
-    <t>&lt;site&gt;/demandes/{bool}</t>
-  </si>
-  <si>
-    <t>&lt;site&gt;/demandes/{string}</t>
-  </si>
-  <si>
-    <t>&lt;site&gt;/conseillers/{id}/demandes/{id}</t>
-  </si>
-  <si>
-    <t>&lt;site&gt;/conseillers/{id}/clients/{id}</t>
-  </si>
-  <si>
-    <t>&lt;site&gt;/conseillers/{id}/clients</t>
-  </si>
-  <si>
     <t>&lt;site&gt;/comptes/{id}</t>
   </si>
   <si>
@@ -235,12 +165,99 @@
   </si>
   <si>
     <t>getNotificationsByClient(clientID)</t>
+  </si>
+  <si>
+    <t>WS</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>&lt;site&gt;/conseillers</t>
+  </si>
+  <si>
+    <t>getAll()</t>
+  </si>
+  <si>
+    <t>WSConseiller</t>
+  </si>
+  <si>
+    <t>WSDemande</t>
+  </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>&lt;site&gt;/conseillers/{recherche}</t>
+  </si>
+  <si>
+    <t>getConseillerByNameOrMatricule(String recherche)</t>
+  </si>
+  <si>
+    <t>updateConseiller(Conseiller conseiller)</t>
+  </si>
+  <si>
+    <t>A revoir</t>
+  </si>
+  <si>
+    <t>&lt;site&gt;/conseillers/{matricule}/clients</t>
+  </si>
+  <si>
+    <t>getClientsFromConseiller(String matricule)</t>
+  </si>
+  <si>
+    <t>addConseiller(Conseiller conseiller)</t>
+  </si>
+  <si>
+    <t>&lt;site&gt;/conseillers/{matricule}</t>
+  </si>
+  <si>
+    <t>deleteConseiller(String matricule)</t>
+  </si>
+  <si>
+    <t>&lt;site&gt;/conseillers/{matricule}/inscriptions</t>
+  </si>
+  <si>
+    <t>getInscriptionsFromConseiller(String matricule)</t>
+  </si>
+  <si>
+    <t>List&lt;DemandeInscription&gt;</t>
+  </si>
+  <si>
+    <t>&lt;site&gt;/conseillers/client/{idClient}</t>
+  </si>
+  <si>
+    <t>getConseillerWithClient(int idClient)</t>
+  </si>
+  <si>
+    <t>&lt;site&gt;/{matricule}/clients/{idClient}</t>
+  </si>
+  <si>
+    <t>deleteClientFromConseiller(int idClient, String matricule)</t>
+  </si>
+  <si>
+    <t>// utile ?</t>
+  </si>
+  <si>
+    <t>&lt;site&gt;/demandes/inscriptions</t>
+  </si>
+  <si>
+    <t>&lt;site&gt;/demandes/inscriptions/{id}</t>
+  </si>
+  <si>
+    <t>DemandeInscription</t>
+  </si>
+  <si>
+    <t>getDemandeInscrById(int id)</t>
+  </si>
+  <si>
+    <t>updateDemandeInscription(DemandeInscription demandeInscr)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -309,21 +326,26 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:E31" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="A1:E31"/>
-  <sortState ref="A2:E28">
-    <sortCondition ref="E1:E28"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:G30" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A1:G30"/>
+  <sortState ref="A2:G27">
+    <sortCondition ref="G1:G27"/>
   </sortState>
-  <tableColumns count="5">
+  <tableColumns count="7">
     <tableColumn id="1" name="VERBE"/>
     <tableColumn id="2" name="PATH"/>
     <tableColumn id="3" name="METHODE"/>
     <tableColumn id="4" name="RETURN"/>
+    <tableColumn id="6" name="WS"/>
+    <tableColumn id="7" name="Test"/>
     <tableColumn id="5" name="COTE"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -373,7 +395,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -406,9 +428,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -441,6 +480,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -617,23 +673,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="29.140625" customWidth="1"/>
-    <col min="2" max="2" width="49.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="48.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34.7109375" customWidth="1"/>
-    <col min="5" max="5" width="21.28515625" customWidth="1"/>
-    <col min="6" max="6" width="20" customWidth="1"/>
+    <col min="1" max="1" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="53.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -647,465 +705,488 @@
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>8</v>
       </c>
       <c r="B2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" t="s">
         <v>51</v>
-      </c>
-      <c r="C2" t="s">
-        <v>49</v>
       </c>
       <c r="D2" t="s">
         <v>5</v>
       </c>
       <c r="E2" t="s">
+        <v>52</v>
+      </c>
+      <c r="F2" t="s">
+        <v>54</v>
+      </c>
+      <c r="G2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" t="s">
+        <v>52</v>
+      </c>
+      <c r="F3" t="s">
+        <v>54</v>
+      </c>
+      <c r="G3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D4" t="s">
         <v>12</v>
       </c>
-      <c r="B4" t="s">
+      <c r="E4" t="s">
         <v>52</v>
       </c>
-      <c r="C4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
+        <v>58</v>
+      </c>
+      <c r="G4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="C5" t="s">
-        <v>18</v>
+        <v>60</v>
       </c>
       <c r="D5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" t="s">
+        <v>52</v>
+      </c>
+      <c r="G5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" t="s">
+        <v>61</v>
+      </c>
+      <c r="D6" t="s">
+        <v>45</v>
+      </c>
+      <c r="E6" t="s">
+        <v>52</v>
+      </c>
+      <c r="G6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>13</v>
       </c>
-      <c r="E5" t="s">
+      <c r="B7" t="s">
+        <v>62</v>
+      </c>
+      <c r="C7" t="s">
+        <v>63</v>
+      </c>
+      <c r="D7" t="s">
+        <v>45</v>
+      </c>
+      <c r="E7" t="s">
+        <v>52</v>
+      </c>
+      <c r="G7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" t="s">
-        <v>53</v>
-      </c>
-      <c r="C6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" t="s">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
+        <v>64</v>
+      </c>
+      <c r="C8" t="s">
+        <v>65</v>
+      </c>
+      <c r="D8" t="s">
+        <v>66</v>
+      </c>
+      <c r="E8" t="s">
+        <v>52</v>
+      </c>
+      <c r="G8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>8</v>
       </c>
-      <c r="B7" t="s">
-        <v>54</v>
-      </c>
-      <c r="C7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" t="s">
+      <c r="B9" t="s">
+        <v>67</v>
+      </c>
+      <c r="C9" t="s">
+        <v>68</v>
+      </c>
+      <c r="D9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" t="s">
+        <v>52</v>
+      </c>
+      <c r="F9" t="s">
+        <v>71</v>
+      </c>
+      <c r="G9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>13</v>
       </c>
-      <c r="E7" t="s">
+      <c r="B10" t="s">
+        <v>69</v>
+      </c>
+      <c r="C10" t="s">
+        <v>70</v>
+      </c>
+      <c r="D10" t="s">
+        <v>45</v>
+      </c>
+      <c r="E10" t="s">
+        <v>52</v>
+      </c>
+      <c r="F10" t="s">
+        <v>71</v>
+      </c>
+      <c r="G10" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" t="s">
-        <v>53</v>
-      </c>
-      <c r="C8" t="s">
-        <v>21</v>
-      </c>
-      <c r="D8" t="s">
-        <v>13</v>
-      </c>
-      <c r="E8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" t="s">
-        <v>53</v>
-      </c>
-      <c r="C9" t="s">
-        <v>22</v>
-      </c>
-      <c r="D9" t="s">
-        <v>16</v>
-      </c>
-      <c r="E9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" t="s">
-        <v>55</v>
-      </c>
-      <c r="C10" t="s">
-        <v>25</v>
-      </c>
-      <c r="D10" t="s">
-        <v>23</v>
-      </c>
-      <c r="E10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11" t="s">
-        <v>56</v>
-      </c>
-      <c r="C11" t="s">
-        <v>24</v>
-      </c>
-      <c r="D11" t="s">
-        <v>23</v>
-      </c>
-      <c r="E11" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>57</v>
+        <v>72</v>
       </c>
       <c r="C12" t="s">
-        <v>26</v>
+        <v>51</v>
       </c>
       <c r="D12" t="s">
-        <v>23</v>
+        <v>66</v>
       </c>
       <c r="E12" t="s">
+        <v>53</v>
+      </c>
+      <c r="G12" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B13" t="s">
-        <v>58</v>
+        <v>73</v>
       </c>
       <c r="C13" t="s">
-        <v>29</v>
+        <v>75</v>
       </c>
       <c r="D13" t="s">
-        <v>16</v>
+        <v>74</v>
       </c>
       <c r="E13" t="s">
+        <v>53</v>
+      </c>
+      <c r="G13" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B14" t="s">
-        <v>58</v>
+        <v>72</v>
       </c>
       <c r="C14" t="s">
-        <v>28</v>
+        <v>76</v>
       </c>
       <c r="D14" t="s">
-        <v>27</v>
+        <v>45</v>
       </c>
       <c r="E14" t="s">
+        <v>53</v>
+      </c>
+      <c r="G14" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>12</v>
-      </c>
-      <c r="B15" t="s">
-        <v>59</v>
-      </c>
-      <c r="C15" t="s">
-        <v>30</v>
-      </c>
-      <c r="D15" t="s">
-        <v>16</v>
-      </c>
-      <c r="E15" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>8</v>
       </c>
       <c r="B16" t="s">
-        <v>60</v>
+        <v>25</v>
       </c>
       <c r="C16" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="D16" t="s">
-        <v>4</v>
-      </c>
-      <c r="E16" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+      <c r="G16" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>8</v>
       </c>
       <c r="B17" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C17" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="D17" t="s">
-        <v>35</v>
-      </c>
-      <c r="E17" t="s">
+        <v>9</v>
+      </c>
+      <c r="G17" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>8</v>
       </c>
       <c r="B18" t="s">
-        <v>62</v>
+        <v>36</v>
       </c>
       <c r="C18" t="s">
+        <v>28</v>
+      </c>
+      <c r="D18" t="s">
+        <v>29</v>
+      </c>
+      <c r="G18" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>8</v>
+      </c>
+      <c r="B20" t="s">
+        <v>38</v>
+      </c>
+      <c r="C20" t="s">
+        <v>31</v>
+      </c>
+      <c r="D20" t="s">
+        <v>32</v>
+      </c>
+      <c r="G20" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>11</v>
+      </c>
+      <c r="B21" t="s">
+        <v>35</v>
+      </c>
+      <c r="C21" t="s">
+        <v>33</v>
+      </c>
+      <c r="D21" t="s">
+        <v>14</v>
+      </c>
+      <c r="G21" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>11</v>
+      </c>
+      <c r="B22" t="s">
+        <v>39</v>
+      </c>
+      <c r="C22" t="s">
+        <v>20</v>
+      </c>
+      <c r="D22" t="s">
+        <v>21</v>
+      </c>
+      <c r="G22" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>15</v>
+      </c>
+      <c r="B23" t="s">
+        <v>39</v>
+      </c>
+      <c r="C23" t="s">
+        <v>23</v>
+      </c>
+      <c r="D23" t="s">
+        <v>14</v>
+      </c>
+      <c r="G23" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>8</v>
+      </c>
+      <c r="B24" t="s">
+        <v>40</v>
+      </c>
+      <c r="C24" t="s">
+        <v>24</v>
+      </c>
+      <c r="D24" t="s">
+        <v>21</v>
+      </c>
+      <c r="G24" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>11</v>
+      </c>
+      <c r="B25" t="s">
+        <v>41</v>
+      </c>
+      <c r="C25" t="s">
+        <v>17</v>
+      </c>
+      <c r="D25" t="s">
+        <v>16</v>
+      </c>
+      <c r="G25" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>11</v>
+      </c>
+      <c r="B26" t="s">
         <v>42</v>
       </c>
-      <c r="D18" t="s">
-        <v>9</v>
-      </c>
-      <c r="E18" t="s">
+      <c r="C26" t="s">
+        <v>34</v>
+      </c>
+      <c r="D26" t="s">
+        <v>19</v>
+      </c>
+      <c r="G26" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>13</v>
+      </c>
+      <c r="B28" t="s">
+        <v>43</v>
+      </c>
+      <c r="C28" t="s">
+        <v>44</v>
+      </c>
+      <c r="D28" t="s">
+        <v>45</v>
+      </c>
+      <c r="G28" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>11</v>
+      </c>
+      <c r="B29" t="s">
+        <v>43</v>
+      </c>
+      <c r="C29" t="s">
+        <v>46</v>
+      </c>
+      <c r="D29" t="s">
+        <v>45</v>
+      </c>
+      <c r="G29" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
         <v>8</v>
       </c>
-      <c r="B19" t="s">
-        <v>61</v>
-      </c>
-      <c r="C19" t="s">
+      <c r="B30" t="s">
         <v>43</v>
       </c>
-      <c r="D19" t="s">
-        <v>44</v>
-      </c>
-      <c r="E19" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>8</v>
-      </c>
-      <c r="B21" t="s">
-        <v>63</v>
-      </c>
-      <c r="C21" t="s">
-        <v>46</v>
-      </c>
-      <c r="D21" t="s">
+      <c r="C30" t="s">
         <v>47</v>
       </c>
-      <c r="E21" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>12</v>
-      </c>
-      <c r="B22" t="s">
-        <v>55</v>
-      </c>
-      <c r="C22" t="s">
-        <v>48</v>
-      </c>
-      <c r="D22" t="s">
-        <v>16</v>
-      </c>
-      <c r="E22" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>12</v>
-      </c>
-      <c r="B23" t="s">
-        <v>64</v>
-      </c>
-      <c r="C23" t="s">
-        <v>34</v>
-      </c>
-      <c r="D23" t="s">
-        <v>35</v>
-      </c>
-      <c r="E23" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>20</v>
-      </c>
-      <c r="B24" t="s">
-        <v>64</v>
-      </c>
-      <c r="C24" t="s">
-        <v>37</v>
-      </c>
-      <c r="D24" t="s">
-        <v>16</v>
-      </c>
-      <c r="E24" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>8</v>
-      </c>
-      <c r="B25" t="s">
-        <v>65</v>
-      </c>
-      <c r="C25" t="s">
-        <v>38</v>
-      </c>
-      <c r="D25" t="s">
-        <v>35</v>
-      </c>
-      <c r="E25" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>12</v>
-      </c>
-      <c r="B26" t="s">
-        <v>66</v>
-      </c>
-      <c r="C26" t="s">
-        <v>31</v>
-      </c>
-      <c r="D26" t="s">
-        <v>27</v>
-      </c>
-      <c r="E26" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>12</v>
-      </c>
-      <c r="B27" t="s">
-        <v>67</v>
-      </c>
-      <c r="C27" t="s">
-        <v>50</v>
-      </c>
-      <c r="D27" t="s">
-        <v>33</v>
-      </c>
-      <c r="E27" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>14</v>
-      </c>
-      <c r="B29" t="s">
-        <v>68</v>
-      </c>
-      <c r="C29" t="s">
-        <v>69</v>
-      </c>
-      <c r="D29" t="s">
-        <v>70</v>
-      </c>
-      <c r="E29" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>12</v>
-      </c>
-      <c r="B30" t="s">
-        <v>68</v>
-      </c>
-      <c r="C30" t="s">
-        <v>71</v>
-      </c>
       <c r="D30" t="s">
-        <v>70</v>
-      </c>
-      <c r="E30" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>8</v>
-      </c>
-      <c r="B31" t="s">
-        <v>68</v>
-      </c>
-      <c r="C31" t="s">
-        <v>72</v>
-      </c>
-      <c r="D31" t="s">
-        <v>45</v>
-      </c>
-      <c r="E31" t="s">
+        <v>30</v>
+      </c>
+      <c r="G30" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1124,7 +1205,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1136,7 +1217,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Vérification des WS (Excel)
</commit_message>
<xml_diff>
--- a/GestiBank/PATHS.xlsx
+++ b/GestiBank/PATHS.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19001"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="60" windowWidth="28512" windowHeight="12840"/>
+    <workbookView xWindow="120" yWindow="60" windowWidth="28512" windowHeight="12840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="75">
   <si>
     <t>VERBE</t>
   </si>
@@ -212,12 +212,6 @@
     <t>deleteConseiller(String matricule)</t>
   </si>
   <si>
-    <t>&lt;site&gt;/conseillers/{matricule}/inscriptions</t>
-  </si>
-  <si>
-    <t>getInscriptionsFromConseiller(String matricule)</t>
-  </si>
-  <si>
     <t>List&lt;DemandeInscription&gt;</t>
   </si>
   <si>
@@ -249,12 +243,15 @@
   </si>
   <si>
     <t>OK (attention à la casse)</t>
+  </si>
+  <si>
+    <t>ne fonctionne pas toujours…</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -331,19 +328,19 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:G30" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="A1:G30"/>
-  <sortState ref="A2:G27">
-    <sortCondition ref="G1:G27"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tableau1" displayName="Tableau1" ref="A1:G29" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A1:G29" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <sortState ref="A2:G26">
+    <sortCondition ref="G1:G26"/>
   </sortState>
   <tableColumns count="7">
-    <tableColumn id="1" name="VERBE"/>
-    <tableColumn id="2" name="PATH"/>
-    <tableColumn id="3" name="METHODE"/>
-    <tableColumn id="4" name="RETURN"/>
-    <tableColumn id="6" name="WS"/>
-    <tableColumn id="7" name="Test"/>
-    <tableColumn id="5" name="COTE"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="VERBE"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="PATH"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="METHODE"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="RETURN"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="WS"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Test"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="COTE"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -669,11 +666,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G30"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -683,7 +680,7 @@
     <col min="3" max="3" width="53.21875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="20" customWidth="1"/>
   </cols>
@@ -751,7 +748,7 @@
         <v>52</v>
       </c>
       <c r="F3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G3" t="s">
         <v>7</v>
@@ -796,6 +793,9 @@
       <c r="E5" t="s">
         <v>52</v>
       </c>
+      <c r="F5" t="s">
+        <v>54</v>
+      </c>
       <c r="G5" t="s">
         <v>7</v>
       </c>
@@ -816,6 +816,9 @@
       <c r="E6" t="s">
         <v>52</v>
       </c>
+      <c r="F6" t="s">
+        <v>54</v>
+      </c>
       <c r="G6" t="s">
         <v>7</v>
       </c>
@@ -836,6 +839,9 @@
       <c r="E7" t="s">
         <v>52</v>
       </c>
+      <c r="F7" t="s">
+        <v>54</v>
+      </c>
       <c r="G7" t="s">
         <v>7</v>
       </c>
@@ -845,24 +851,27 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C8" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D8" t="s">
-        <v>65</v>
+        <v>12</v>
       </c>
       <c r="E8" t="s">
         <v>52</v>
       </c>
+      <c r="F8" t="s">
+        <v>54</v>
+      </c>
       <c r="G8" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="B9" t="s">
         <v>66</v>
@@ -871,32 +880,38 @@
         <v>67</v>
       </c>
       <c r="D9" t="s">
-        <v>12</v>
+        <v>45</v>
       </c>
       <c r="E9" t="s">
         <v>52</v>
       </c>
+      <c r="F9" t="s">
+        <v>74</v>
+      </c>
       <c r="G9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" t="s">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" t="s">
         <v>68</v>
       </c>
-      <c r="C10" t="s">
-        <v>69</v>
-      </c>
-      <c r="D10" t="s">
-        <v>45</v>
-      </c>
-      <c r="E10" t="s">
-        <v>52</v>
-      </c>
-      <c r="G10" t="s">
+      <c r="C11" t="s">
+        <v>51</v>
+      </c>
+      <c r="D11" t="s">
+        <v>63</v>
+      </c>
+      <c r="E11" t="s">
+        <v>53</v>
+      </c>
+      <c r="F11" t="s">
+        <v>54</v>
+      </c>
+      <c r="G11" t="s">
         <v>7</v>
       </c>
     </row>
@@ -905,59 +920,62 @@
         <v>8</v>
       </c>
       <c r="B12" t="s">
+        <v>69</v>
+      </c>
+      <c r="C12" t="s">
+        <v>71</v>
+      </c>
+      <c r="D12" t="s">
         <v>70</v>
-      </c>
-      <c r="C12" t="s">
-        <v>51</v>
-      </c>
-      <c r="D12" t="s">
-        <v>65</v>
       </c>
       <c r="E12" t="s">
         <v>53</v>
       </c>
+      <c r="F12" t="s">
+        <v>54</v>
+      </c>
       <c r="G12" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="B13" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C13" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D13" t="s">
-        <v>72</v>
+        <v>45</v>
       </c>
       <c r="E13" t="s">
         <v>53</v>
       </c>
+      <c r="F13" t="s">
+        <v>54</v>
+      </c>
       <c r="G13" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>15</v>
-      </c>
-      <c r="B14" t="s">
-        <v>70</v>
-      </c>
-      <c r="C14" t="s">
-        <v>74</v>
-      </c>
-      <c r="D14" t="s">
-        <v>45</v>
-      </c>
-      <c r="E14" t="s">
-        <v>53</v>
-      </c>
-      <c r="G14" t="s">
-        <v>7</v>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" t="s">
+        <v>26</v>
+      </c>
+      <c r="D15" t="s">
+        <v>21</v>
+      </c>
+      <c r="G15" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
@@ -965,13 +983,13 @@
         <v>8</v>
       </c>
       <c r="B16" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="C16" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D16" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="G16" t="s">
         <v>10</v>
@@ -982,47 +1000,47 @@
         <v>8</v>
       </c>
       <c r="B17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C17" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D17" t="s">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="G17" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
         <v>8</v>
       </c>
-      <c r="B18" t="s">
-        <v>36</v>
-      </c>
-      <c r="C18" t="s">
-        <v>28</v>
-      </c>
-      <c r="D18" t="s">
-        <v>29</v>
-      </c>
-      <c r="G18" t="s">
+      <c r="B19" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19" t="s">
+        <v>31</v>
+      </c>
+      <c r="D19" t="s">
+        <v>32</v>
+      </c>
+      <c r="G19" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B20" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C20" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D20" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="G20" t="s">
         <v>10</v>
@@ -1033,30 +1051,30 @@
         <v>11</v>
       </c>
       <c r="B21" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="C21" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="D21" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="G21" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B22" t="s">
         <v>39</v>
       </c>
       <c r="C22" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D22" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="G22" t="s">
         <v>22</v>
@@ -1064,16 +1082,16 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="B23" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C23" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D23" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="G23" t="s">
         <v>22</v>
@@ -1081,19 +1099,19 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B24" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C24" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="D24" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="G24" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
@@ -1101,44 +1119,44 @@
         <v>11</v>
       </c>
       <c r="B25" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C25" t="s">
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="D25" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="G25" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>11</v>
-      </c>
-      <c r="B26" t="s">
-        <v>42</v>
-      </c>
-      <c r="C26" t="s">
-        <v>34</v>
-      </c>
-      <c r="D26" t="s">
-        <v>19</v>
-      </c>
-      <c r="G26" t="s">
-        <v>18</v>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>13</v>
+      </c>
+      <c r="B27" t="s">
+        <v>43</v>
+      </c>
+      <c r="C27" t="s">
+        <v>44</v>
+      </c>
+      <c r="D27" t="s">
+        <v>45</v>
+      </c>
+      <c r="G27" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B28" t="s">
         <v>43</v>
       </c>
       <c r="C28" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D28" t="s">
         <v>45</v>
@@ -1149,35 +1167,18 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B29" t="s">
         <v>43</v>
       </c>
       <c r="C29" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D29" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="G29" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>8</v>
-      </c>
-      <c r="B30" t="s">
-        <v>43</v>
-      </c>
-      <c r="C30" t="s">
-        <v>47</v>
-      </c>
-      <c r="D30" t="s">
-        <v>30</v>
-      </c>
-      <c r="G30" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1191,7 +1192,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1203,7 +1204,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>